<commit_message>
Excel files changed to correct 1 poster, 1 symposium
</commit_message>
<xml_diff>
--- a/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
+++ b/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gluth/Arbeit/Conferences_Talks/PuG2024/PuG_2024_Booklet/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48346D5-E40B-024D-BB6F-44467ECC5619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFDBAA6-28AF-D14F-87C2-C62D8688B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35880" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{50F79AB2-BE02-9945-951E-3A2C179FFBAC}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="34780" windowHeight="21900" xr2:uid="{50F79AB2-BE02-9945-951E-3A2C179FFBAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14739,9 +14739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB778129-3AB6-F845-A6EE-0C2E52353F3C}">
   <dimension ref="A1:M196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I183" sqref="I183"/>
+      <selection pane="bottomLeft" activeCell="M183" sqref="M183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21685,7 +21685,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="184" spans="1:13" s="10" customFormat="1" ht="333" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" s="10" customFormat="1" ht="350" x14ac:dyDescent="0.2">
       <c r="A184" s="10" t="s">
         <v>29</v>
       </c>
@@ -21726,7 +21726,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="185" spans="1:13" s="10" customFormat="1" ht="296" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" s="10" customFormat="1" ht="316" x14ac:dyDescent="0.2">
       <c r="A185" s="10" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
updates on excel files (esp. posters)
</commit_message>
<xml_diff>
--- a/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
+++ b/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gluth/Arbeit/Conferences_Talks/PuG2024/PuG_2024_Booklet/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{461B5829-DBE0-4294-9E15-37651B86386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8410A1EC-C8B2-4D39-A034-DEC45008A143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35880" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{50F79AB2-BE02-9945-951E-3A2C179FFBAC}"/>
   </bookViews>
@@ -4836,7 +4836,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Thu-$$-Talk-$-$$$
@@ -4846,7 +4846,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
@@ -4857,7 +4857,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Philipps-Universität Marburg
@@ -4866,7 +4866,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
@@ -4888,7 +4888,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Thu-$$-Talk-$-$$$
@@ -4898,7 +4898,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
@@ -4909,7 +4909,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Universität Mannheim
@@ -4918,7 +4918,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
@@ -4936,7 +4936,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -4947,7 +4947,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -4959,7 +4959,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -4969,7 +4969,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -4988,7 +4988,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -4999,7 +4999,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5011,7 +5011,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5021,7 +5021,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5030,6 +5030,217 @@
     </r>
   </si>
   <si>
+    <t>Roman Kessler</t>
+  </si>
+  <si>
+    <t>Max-Planck-Institut für Kognitions- und Neurowissenschaften Leipzig</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thu-$$-Talk-$-$$$
+Is EEG better left alone for decoding?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Roman Kessler (1)
+(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Max-Planck-Institut für Kognitions- und Neurowissenschaften Leipzig
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Multiverse preprocessing has revealed the effect of single data preprocessing choices on ERP amplitude or latency. In multiverse approaches, pipelines are systematically varied, and downstream analyses are compared between forking paths (i.e., universes), providing insights into stability, generalizability, and the impact of researchers’ degrees of freedom on analysis outcomes. One particular use case is EEG decoding which exploits the multidimensionality of the data corresponding to specific cognitive processes to provide insight into how neural representations of categories differ or evolve over time.
+The objective of this study is to investigate the effect of preprocessing choices on the performance of decoding algorithms using multiverse preprocessing. The open ERPCORE dataset comprising different experiments was analyzed (ERN, LRP, MMN, N170, N2pc, N400, P3). We systematically varied each preprocessing step, including filtering, re-referencing, eye/muscle artifact correction, interpolations, and epoching. Decoding was performed based on each universe, either trial-wise using deep neural networks or time-resolved using logistic regression. 
+The results indicate that there are systematic but small performance differences between universes when using neural networks. This suggests that their filters are successfully learned independent of the preprocessing. However, for time-resolved decoding, performance differences were larger, with stringent filtering being the most important for achieving high decoding performance. Additionally, most artifact correction steps rather decreased decoding performance in both model types.
+The present study suggests that EEG preprocessing steps, beyond filtering, can reduce model accuracy. Additionally, our work suggests that the impact of preprocessing steps heavily depends on the decoding algorithm, as well as the experiment.</t>
+    </r>
+  </si>
+  <si>
+    <t>Linn Petersdotter</t>
+  </si>
+  <si>
+    <t>Lund University</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thu-$$-Talk-$-$$$
+Deciphering the impact of a trauma analogue - the roles of peritraumatic response, inhibitory control and memory reactivation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Linn Petersdotter (1)
+(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lund University
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Hitherto, it remains poorly understood why some trauma survivors develop post traumatic symptoms leading to mental health conditions while others do not. The aim of this study was to increase the understanding of which mechanisms may underlie variability in trauma related symptom development. Using a trauma-analogue film paradigm in a healthy sample (N = 33), we investigated how heartrate during trauma film exposure, individual inhibitory control capacity and the experienced impact of the trauma-analogue (IES) relate to intrusive memory development over the course of a week. Further, we tested the effect of trauma reminders on task performance in a 24-hour delayed cognitive control task. We found that lower inhibitory control and increased heartrate during trauma film exposure were related to both higher IES scores and intrusive memory frequencies. In a task with high cognitive control demands, negative trauma reminders led to significantly longer reaction latencies compared to their neutral counterparts while the opposite was true for negative non-reminders. To further understand the potential impact of subjective trauma experience, a median split into high and low IES scores was performed, showing that the effect of diminished cognitive control for negative trauma reminders was mainly driven by the highly impacted group. Our study extends previous research by providing deeper insights into how individual experiences of trauma-analogue exposure, heartrate, and the role of inhibitory control are related to the development of intrusive memories, and the resolution of cognitive interference when faced with trauma relevant reminders.</t>
+    </r>
+  </si>
+  <si>
+    <t>Nicole Rheinheimer</t>
+  </si>
+  <si>
+    <t>Radboudumc Nijmegen</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thu-$$-Talk-$-$$$
+Associations of Infant Colic with Sleeping Problems from Childhood through Adolescence
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Nicole Rheinheimer (1)
+(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Radboudumc Nijmegen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Colic is characterized by high levels of unsoothable crying for more than three hours daily, peaking around six weeks postpartum. Studies suggest a high prevalence of sleeping problems in colicky infants with problems reaching up to 10 years of age. Many of the previous studies, however, relied on unstandardized and retrospective maternal recall, and no studies to date have followed colicky infants beyond the age of 10. Therefore, the aim of this study is to investigate the association of infant colic with reported sleeping problems from 2.5 until 16 years of age, as well as polysomnography at age 16. In this longitudinal study on a community sample, colic was diagnosed using prospective cry-diaries, filled in by the mothers for 4 days at age 6 weeks. Sleeping problems were assessed using maternal report at ages 2.5, 6 and 10 years, and child self-report at ages 12.5, 14 and 16 years. At age 16, 7 days of polysomnography data were collected using EEG wearables at home (Hypnodyne Corp., Sofia, Bulgaria). The research data is currently being analyzed and results will be presented at the conference.</t>
+    </r>
+  </si>
+  <si>
+    <t>Leon Kroczek</t>
+  </si>
+  <si>
+    <t>Universität Regensburg</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Thu-$$-Talk-$-$$$
+Communicative social intentions modulate emotional mimicry responses
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Leon Kroczek (1)
+(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Universität Regensburg
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The coordinated exchange of facial expressions is an important part of face-to-face social interactions. Previous research has shown that sending a facial emotional expression influences the evaluation of response expressions, but it remains unclear whether this effect is driven by the display of the facial expression or rather by the communicative intention. In a preregistered experiment, 68 participants were asked to send an emoji (smiley, neutral, frowny) via a computer display to a virtual agent in front of them, whereupon the agent reacted with either a smiling or frowning facial expression. Mimicry responses were measured via facial EMG of the Zygomaticus and Corrugator muscle following the agent’s response. In addition, valence and arousal ratings were obtained after the interactive exchange. The results show that being smiled at is more pleasant and elicits greater Zygomaticus activation when the smile is received as a response to a smile emoji compared to a neutral or frown emoji. Interestingly, a mirrored pattern but with a smaller effect size was observed when participants were being frowned at, i.e. an agent’s frown was less pleasant and elicited greater Corrugator activation when it followed a smile emoji compared to a frown emoji. The results demonstrate that communicative intentions are sufficient to change the evaluation of facial response expressions of an interactive partner and that persons are sensitive to the congruency in emotional signals between sender and receiver. Using a minimal social interaction paradigm, the present study highlights interactive mechanisms in the evaluation of facial emotions.</t>
+    </r>
+  </si>
+  <si>
     <t>Kim M. Sobania</t>
   </si>
   <si>
@@ -5037,7 +5248,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5048,7 +5259,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5060,7 +5271,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5070,7 +5281,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -5079,217 +5290,6 @@
 In the current study, we investigated the late positive potential (LPP), fear-potentiated startle data (FPS), and behavioral data (US-expectancy ratings) in a large transdiagnostic sample of participants with OCD (n=38), social phobia (n=39), specific phobia (n=40), and healthy controls (n=39). A differential fear generalization paradigm was employed, including a habituation, acquisition, generalization, and extinction phase. Geometrical forms were utilized, with one color consistently paired with aversive electrical stimulation (CS+), while another color remained unpaired (CS-). Three colors in between the CS+ and CS- served as generalization stimuli.
 Behavioral, LPP, and FPS data indicated a successful fear acquisition, which was generalized to the stimulus most similar in color to the CS+. Although a reduction for the CS+ was visible during extinction for behavioral and FPS data, it remained significantly higher compared to the CS-. For the LPP, no differences during extinction were found. However, results revealed no differences between any diagnostic groups.
 The present results suggest that both, behavioral and neural data, reflect fear learning. Nevertheless, the unexpected absence of differences between the groups suggests a necessity for further studies to elucidate the involved fear learning mechanisms among individuals with OCD and anxiety patients.</t>
-    </r>
-  </si>
-  <si>
-    <t>Linn Petersdotter</t>
-  </si>
-  <si>
-    <t>Lund University</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Thu-$$-Talk-$-$$$
-Deciphering the impact of a trauma analogue - the roles of peritraumatic response, inhibitory control and memory reactivation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Linn Petersdotter (1)
-(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Lund University
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Hitherto, it remains poorly understood why some trauma survivors develop post traumatic symptoms leading to mental health conditions while others do not. The aim of this study was to increase the understanding of which mechanisms may underlie variability in trauma related symptom development. Using a trauma-analogue film paradigm in a healthy sample (N = 33), we investigated how heartrate during trauma film exposure, individual inhibitory control capacity and the experienced impact of the trauma-analogue (IES) relate to intrusive memory development over the course of a week. Further, we tested the effect of trauma reminders on task performance in a 24-hour delayed cognitive control task. We found that lower inhibitory control and increased heartrate during trauma film exposure were related to both higher IES scores and intrusive memory frequencies. In a task with high cognitive control demands, negative trauma reminders led to significantly longer reaction latencies compared to their neutral counterparts while the opposite was true for negative non-reminders. To further understand the potential impact of subjective trauma experience, a median split into high and low IES scores was performed, showing that the effect of diminished cognitive control for negative trauma reminders was mainly driven by the highly impacted group. Our study extends previous research by providing deeper insights into how individual experiences of trauma-analogue exposure, heartrate, and the role of inhibitory control are related to the development of intrusive memories, and the resolution of cognitive interference when faced with trauma relevant reminders.</t>
-    </r>
-  </si>
-  <si>
-    <t>Nicole Rheinheimer</t>
-  </si>
-  <si>
-    <t>Radboudumc Nijmegen</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Thu-$$-Talk-$-$$$
-Associations of Infant Colic with Sleeping Problems from Childhood through Adolescence
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Nicole Rheinheimer (1)
-(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Radboudumc Nijmegen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Colic is characterized by high levels of unsoothable crying for more than three hours daily, peaking around six weeks postpartum. Studies suggest a high prevalence of sleeping problems in colicky infants with problems reaching up to 10 years of age. Many of the previous studies, however, relied on unstandardized and retrospective maternal recall, and no studies to date have followed colicky infants beyond the age of 10. Therefore, the aim of this study is to investigate the association of infant colic with reported sleeping problems from 2.5 until 16 years of age, as well as polysomnography at age 16. In this longitudinal study on a community sample, colic was diagnosed using prospective cry-diaries, filled in by the mothers for 4 days at age 6 weeks. Sleeping problems were assessed using maternal report at ages 2.5, 6 and 10 years, and child self-report at ages 12.5, 14 and 16 years. At age 16, 7 days of polysomnography data were collected using EEG wearables at home (Hypnodyne Corp., Sofia, Bulgaria). The research data is currently being analyzed and results will be presented at the conference.</t>
-    </r>
-  </si>
-  <si>
-    <t>Leon Kroczek</t>
-  </si>
-  <si>
-    <t>Universität Regensburg</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Thu-$$-Talk-$-$$$
-Communicative social intentions modulate emotional mimicry responses
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Leon Kroczek (1)
-(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Universität Regensburg
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The coordinated exchange of facial expressions is an important part of face-to-face social interactions. Previous research has shown that sending a facial emotional expression influences the evaluation of response expressions, but it remains unclear whether this effect is driven by the display of the facial expression or rather by the communicative intention. In a preregistered experiment, 68 participants were asked to send an emoji (smiley, neutral, frowny) via a computer display to a virtual agent in front of them, whereupon the agent reacted with either a smiling or frowning facial expression. Mimicry responses were measured via facial EMG of the Zygomaticus and Corrugator muscle following the agent’s response. In addition, valence and arousal ratings were obtained after the interactive exchange. The results show that being smiled at is more pleasant and elicits greater Zygomaticus activation when the smile is received as a response to a smile emoji compared to a neutral or frown emoji. Interestingly, a mirrored pattern but with a smaller effect size was observed when participants were being frowned at, i.e. an agent’s frown was less pleasant and elicited greater Corrugator activation when it followed a smile emoji compared to a frown emoji. The results demonstrate that communicative intentions are sufficient to change the evaluation of facial response expressions of an interactive partner and that persons are sensitive to the congruency in emotional signals between sender and receiver. Using a minimal social interaction paradigm, the present study highlights interactive mechanisms in the evaluation of facial emotions.</t>
-    </r>
-  </si>
-  <si>
-    <t>Roman Kessler</t>
-  </si>
-  <si>
-    <t>Max-Planck-Institut für Kognitions- und Neurowissenschaften Leipzig</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Thu-$$-Talk-$-$$$
-Is EEG better left alone for decoding?
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Roman Kessler (1)
-(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Max-Planck-Institut für Kognitions- und Neurowissenschaften Leipzig
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Multiverse preprocessing has revealed the effect of single data preprocessing choices on ERP amplitude or latency. In multiverse approaches, pipelines are systematically varied, and downstream analyses are compared between forking paths (i.e., universes), providing insights into stability, generalizability, and the impact of researchers’ degrees of freedom on analysis outcomes. One particular use case is EEG decoding which exploits the multidimensionality of the data corresponding to specific cognitive processes to provide insight into how neural representations of categories differ or evolve over time.
-The objective of this study is to investigate the effect of preprocessing choices on the performance of decoding algorithms using multiverse preprocessing. The open ERPCORE dataset comprising different experiments was analyzed (ERN, LRP, MMN, N170, N2pc, N400, P3). We systematically varied each preprocessing step, including filtering, re-referencing, eye/muscle artifact correction, interpolations, and epoching. Decoding was performed based on each universe, either trial-wise using deep neural networks or time-resolved using logistic regression. 
-The results indicate that there are systematic but small performance differences between universes when using neural networks. This suggests that their filters are successfully learned independent of the preprocessing. However, for time-resolved decoding, performance differences were larger, with stringent filtering being the most important for achieving high decoding performance. Additionally, most artifact correction steps rather decreased decoding performance in both model types.
-The present study suggests that EEG preprocessing steps, beyond filtering, can reduce model accuracy. Additionally, our work suggests that the impact of preprocessing steps heavily depends on the decoding algorithm, as well as the experiment.</t>
     </r>
   </si>
   <si>
@@ -13425,7 +13425,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13437,7 +13437,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13450,7 +13450,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13460,7 +13460,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13471,7 +13471,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13481,7 +13481,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13492,7 +13492,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13502,7 +13502,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13513,7 +13513,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13523,7 +13523,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13534,7 +13534,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13554,7 +13554,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13566,7 +13566,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13579,7 +13579,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13589,7 +13589,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13600,7 +13600,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13610,7 +13610,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13621,7 +13621,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13631,7 +13631,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13642,7 +13642,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13652,7 +13652,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -13672,7 +13672,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13683,7 +13683,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13695,7 +13695,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13712,7 +13712,7 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13723,7 +13723,7 @@
     <r>
       <rPr>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13735,7 +13735,7 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -13745,7 +13745,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -14645,7 +14645,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -14785,74 +14785,51 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -14891,7 +14868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -14971,23 +14948,19 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -15310,8 +15283,8 @@
   <dimension ref="A1:N197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -17369,7 +17342,7 @@
       <c r="H55" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="I55" s="5" t="s">
         <v>200</v>
       </c>
       <c r="J55" s="3" t="s">
@@ -17381,7 +17354,7 @@
       <c r="L55" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="M55" s="31" t="s">
+      <c r="M55" s="27" t="s">
         <v>204</v>
       </c>
       <c r="N55" s="19"/>
@@ -17411,7 +17384,7 @@
       <c r="H56" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I56" s="33" t="s">
+      <c r="I56" s="29" t="s">
         <v>205</v>
       </c>
       <c r="J56" s="3" t="s">
@@ -17423,7 +17396,7 @@
       <c r="L56" t="s">
         <v>206</v>
       </c>
-      <c r="M56" s="32" t="s">
+      <c r="M56" s="30" t="s">
         <v>207</v>
       </c>
       <c r="N56" s="19"/>
@@ -17453,7 +17426,7 @@
       <c r="H57" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I57" s="30" t="s">
+      <c r="I57" t="s">
         <v>208</v>
       </c>
       <c r="J57" s="3" t="s">
@@ -17465,7 +17438,7 @@
       <c r="L57" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="M57" s="32" t="s">
+      <c r="M57" s="30" t="s">
         <v>210</v>
       </c>
       <c r="N57" s="19"/>
@@ -17495,7 +17468,7 @@
       <c r="H58" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I58" s="30" t="s">
+      <c r="I58" t="s">
         <v>211</v>
       </c>
       <c r="J58" s="3" t="s">
@@ -17507,7 +17480,7 @@
       <c r="L58" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="M58" s="17" t="s">
+      <c r="M58" s="3" t="s">
         <v>213</v>
       </c>
       <c r="N58" s="19"/>
@@ -17537,7 +17510,7 @@
       <c r="H59" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I59" s="30" t="s">
+      <c r="I59" t="s">
         <v>214</v>
       </c>
       <c r="J59" s="3" t="s">
@@ -17549,7 +17522,7 @@
       <c r="L59" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M59" s="17" t="s">
+      <c r="M59" s="3" t="s">
         <v>216</v>
       </c>
       <c r="N59" s="19"/>
@@ -17568,10 +17541,10 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E60" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.6694444444444444</v>
       </c>
       <c r="F60" s="6">
-        <v>0.65208333333333335</v>
+        <v>0.67569444444444449</v>
       </c>
       <c r="G60" s="25" t="s">
         <v>22</v>
@@ -17579,7 +17552,7 @@
       <c r="H60" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I60" s="30" t="s">
+      <c r="I60" t="s">
         <v>217</v>
       </c>
       <c r="J60" s="3" t="s">
@@ -17588,11 +17561,11 @@
       <c r="K60" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="M60" s="17" t="s">
+      <c r="L60" t="s">
         <v>218</v>
+      </c>
+      <c r="M60" s="31" t="s">
+        <v>219</v>
       </c>
       <c r="N60" s="19"/>
     </row>
@@ -17621,8 +17594,8 @@
       <c r="H61" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I61" s="30" t="s">
-        <v>219</v>
+      <c r="I61" t="s">
+        <v>220</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>201</v>
@@ -17631,10 +17604,10 @@
         <v>202</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="M61" s="17" t="s">
         <v>221</v>
+      </c>
+      <c r="M61" s="31" t="s">
+        <v>222</v>
       </c>
       <c r="N61" s="19"/>
     </row>
@@ -17663,8 +17636,8 @@
       <c r="H62" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I62" s="30" t="s">
-        <v>222</v>
+      <c r="I62" t="s">
+        <v>223</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>201</v>
@@ -17673,10 +17646,10 @@
         <v>202</v>
       </c>
       <c r="L62" t="s">
-        <v>223</v>
-      </c>
-      <c r="M62" s="17" t="s">
         <v>224</v>
+      </c>
+      <c r="M62" s="31" t="s">
+        <v>225</v>
       </c>
       <c r="N62" s="19"/>
     </row>
@@ -17705,8 +17678,8 @@
       <c r="H63" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I63" s="30" t="s">
-        <v>225</v>
+      <c r="I63" t="s">
+        <v>226</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>201</v>
@@ -17715,10 +17688,10 @@
         <v>202</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="M63" s="17" t="s">
         <v>227</v>
+      </c>
+      <c r="M63" s="31" t="s">
+        <v>228</v>
       </c>
       <c r="N63" s="19"/>
     </row>
@@ -17736,10 +17709,10 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E64" s="6">
-        <v>0.6694444444444444</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F64" s="6">
-        <v>0.67569444444444449</v>
+        <v>0.65208333333333335</v>
       </c>
       <c r="G64" s="25" t="s">
         <v>22</v>
@@ -17747,8 +17720,8 @@
       <c r="H64" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I64" s="30" t="s">
-        <v>228</v>
+      <c r="I64" t="s">
+        <v>229</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>201</v>
@@ -17756,10 +17729,10 @@
       <c r="K64" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="L64" t="s">
-        <v>229</v>
-      </c>
-      <c r="M64" s="17" t="s">
+      <c r="L64" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="M64" s="31" t="s">
         <v>230</v>
       </c>
       <c r="N64" s="19"/>
@@ -22173,7 +22146,7 @@
       <c r="H181" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="I181" s="27" t="s">
+      <c r="I181" s="10" t="s">
         <v>615</v>
       </c>
       <c r="J181" s="14" t="s">
@@ -22182,10 +22155,10 @@
       <c r="K181" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="L181" s="27" t="s">
+      <c r="L181" s="10" t="s">
         <v>618</v>
       </c>
-      <c r="M181" s="28" t="s">
+      <c r="M181" s="14" t="s">
         <v>619</v>
       </c>
     </row>
@@ -22214,7 +22187,7 @@
       <c r="H182" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="I182" s="27" t="s">
+      <c r="I182" s="10" t="s">
         <v>620</v>
       </c>
       <c r="J182" s="14" t="s">
@@ -22223,10 +22196,10 @@
       <c r="K182" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="L182" s="27" t="s">
+      <c r="L182" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="M182" s="28" t="s">
+      <c r="M182" s="14" t="s">
         <v>622</v>
       </c>
     </row>
@@ -22255,7 +22228,7 @@
       <c r="H183" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="I183" s="27" t="s">
+      <c r="I183" s="10" t="s">
         <v>623</v>
       </c>
       <c r="J183" s="14" t="s">
@@ -22264,10 +22237,10 @@
       <c r="K183" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="L183" s="27" t="s">
+      <c r="L183" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="M183" s="29" t="s">
+      <c r="M183" s="28" t="s">
         <v>625</v>
       </c>
     </row>
@@ -22296,7 +22269,7 @@
       <c r="H184" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="I184" s="27" t="s">
+      <c r="I184" s="10" t="s">
         <v>626</v>
       </c>
       <c r="J184" s="14" t="s">
@@ -22305,10 +22278,10 @@
       <c r="K184" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="L184" s="27" t="s">
+      <c r="L184" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="M184" s="29" t="s">
+      <c r="M184" s="28" t="s">
         <v>627</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cancellation of a talk
</commit_message>
<xml_diff>
--- a/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
+++ b/data/excel/PUG_2024_Programm_TalksRooms_1905.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurt\Nextcloud\Uni\shk\Booklet\pug24\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gluth/Arbeit/Conferences_Talks/PuG2024/PuG_2024_Booklet/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77D65A94-5959-40A7-B472-07A652683019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B37F2EE0-F5E2-4CE9-AA49-549C29447E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="1910" windowWidth="29920" windowHeight="18230" xr2:uid="{50F79AB2-BE02-9945-951E-3A2C179FFBAC}"/>
+    <workbookView xWindow="35880" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{50F79AB2-BE02-9945-951E-3A2C179FFBAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11144,21 +11144,18 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fri-$$-Talk-$-$$$
-Dissociating the roles of automatic episodic retrieval and contingency awareness in contingency learning</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Fri-$$-Talk-$-$$$
+TALK CANCELLED - Dissociating the roles of automatic episodic retrieval and contingency awareness in contingency learning
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
 Matthäus Rudolph (1), Carina G. Giesen (2)
@@ -11168,20 +11165,16 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t>Friedrich-Schiller-Universität Jena</t>
     </r>
     <r>
       <rPr>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">, (2) </t>
     </r>
@@ -11189,20 +11182,17 @@
       <rPr>
         <i/>
         <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Health and Medical University Erfurt</t>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Health and Medical University Erfurt
+</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
 When we perceive a stimulus, we may respond in a multitude of ways. Often, however, our behavior is not as variable as we would assume. Instead, there is a high likelihood that our current response will equal the response we gave on the last previous occurrence of the very same stimulus. This principle is captured in the law of recency (Giesen et al., 2020), which posits that action control processes often rely on retrieval of previous stimulus-response (SR) episodes from memory. Episodic retrieval will activate the response that was executed during the most recent episode in which the stimulus was presented before. Within the present talk, we will first provide evidence that recency retrieval of SR episodes explains a large part of color-word contingency learning (CL) effects. Still, after controlling for recency retrieval, a residual CL effect remains, which reflects the impact of global contingencies on behavior. Hence, in a second step, we will present data in which we tested the influence of contingency awareness on this residual CL effect by giving true or false instructions about the existing color-word contingencies. We found that the residual CL effect is modulated by awareness, as true (false) instructions amplified (reduced) the residual CL effect. Collectively, our findings suggest that color-word contingency learning is driven by two independent sources: (1) recency-based episodic retrieval which emerges by mere spatial temporal contiguity, and (2) application of contingency knowledge.</t>
@@ -14702,7 +14692,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="36">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -14915,6 +14905,28 @@
       <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -14951,7 +14963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -15055,6 +15067,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -15078,9 +15093,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -15118,7 +15133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -15224,7 +15239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -15366,7 +15381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15377,27 +15392,27 @@
   <dimension ref="A1:N197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M97" sqref="M97"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M153" sqref="M153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="16.83203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="21.08203125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="10.875" style="1"/>
+    <col min="7" max="7" width="16.875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="21.125" style="2" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="19.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.875" style="1"/>
     <col min="13" max="13" width="22.5" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="5"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="10.875" style="5"/>
+    <col min="15" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15441,7 +15456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -15455,7 +15470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -15469,7 +15484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -15486,7 +15501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -15500,7 +15515,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -15514,7 +15529,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="48" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -15558,7 +15573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="90" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -15599,7 +15614,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="215.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="215.1" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -15640,7 +15655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="215.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="215.1" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -15681,7 +15696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="215.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="215.1" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -15722,7 +15737,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="214" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="213.95" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -15766,7 +15781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="214" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="213.95" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -15807,7 +15822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="214" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="213.95" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -15848,7 +15863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="214" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="213.95" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -15889,7 +15904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="225.95" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -15933,7 +15948,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="225.95" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -15974,7 +15989,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="225.95" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -16015,7 +16030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="225.95" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -16056,7 +16071,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="226" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="225.95" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -16097,7 +16112,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="409.6">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -16141,7 +16156,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="409.6">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -16182,7 +16197,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="409.6">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -16223,7 +16238,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="409.6">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -16264,7 +16279,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="409.6">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -16305,7 +16320,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="409.6">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -16349,7 +16364,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="409.6">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -16390,7 +16405,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="409.6">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -16431,7 +16446,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="409.6">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -16472,7 +16487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -16487,7 +16502,7 @@
       </c>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="210" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -16531,7 +16546,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="210" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -16572,7 +16587,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="210" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -16613,7 +16628,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="210" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -16654,7 +16669,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="210" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="210" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -16695,7 +16710,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="409.6">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -16739,7 +16754,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="409.6">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -16780,7 +16795,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="409.6">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -16821,7 +16836,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="409.6">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -16862,7 +16877,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A41" s="10" t="s">
         <v>19</v>
       </c>
@@ -16906,7 +16921,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A42" s="10" t="s">
         <v>19</v>
       </c>
@@ -16948,7 +16963,7 @@
       </c>
       <c r="N42" s="32"/>
     </row>
-    <row r="43" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A43" s="10" t="s">
         <v>19</v>
       </c>
@@ -16990,7 +17005,7 @@
       </c>
       <c r="N43" s="32"/>
     </row>
-    <row r="44" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -17032,7 +17047,7 @@
       </c>
       <c r="N44" s="32"/>
     </row>
-    <row r="45" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="409.6">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -17076,7 +17091,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="409.6">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -17117,7 +17132,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="409.6">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -17158,7 +17173,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="409.6">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -17199,7 +17214,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" ht="409.6">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
@@ -17240,7 +17255,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" ht="245.1" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
@@ -17284,7 +17299,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" ht="245.1" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>19</v>
       </c>
@@ -17325,7 +17340,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" ht="245.1" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>19</v>
       </c>
@@ -17366,7 +17381,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" ht="245.1" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>19</v>
       </c>
@@ -17407,7 +17422,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" ht="245.1" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
@@ -17448,7 +17463,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" ht="245.1" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>19</v>
       </c>
@@ -17492,7 +17507,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" ht="245.1" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>19</v>
       </c>
@@ -17533,7 +17548,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" ht="245.1" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
@@ -17574,7 +17589,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" ht="245.1" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>19</v>
       </c>
@@ -17615,7 +17630,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" ht="245.1" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>19</v>
       </c>
@@ -17656,7 +17671,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" ht="245.1" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>19</v>
       </c>
@@ -17697,7 +17712,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" ht="245.1" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
@@ -17738,7 +17753,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" ht="245.1" customHeight="1">
       <c r="A62" s="1" t="s">
         <v>19</v>
       </c>
@@ -17779,7 +17794,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" ht="245.1" customHeight="1">
       <c r="A63" s="1" t="s">
         <v>19</v>
       </c>
@@ -17820,7 +17835,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="245.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" ht="245.1" customHeight="1">
       <c r="A64" s="1" t="s">
         <v>19</v>
       </c>
@@ -17861,7 +17876,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="409.6">
       <c r="A65" s="1" t="s">
         <v>19</v>
       </c>
@@ -17905,7 +17920,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" ht="409.6">
       <c r="A66" s="1" t="s">
         <v>19</v>
       </c>
@@ -17946,7 +17961,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" ht="409.6">
       <c r="A67" s="1" t="s">
         <v>19</v>
       </c>
@@ -17987,7 +18002,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" ht="409.6">
       <c r="A68" s="1" t="s">
         <v>19</v>
       </c>
@@ -18028,7 +18043,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" ht="409.6">
       <c r="A69" s="1" t="s">
         <v>19</v>
       </c>
@@ -18072,7 +18087,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" ht="409.6">
       <c r="A70" s="1" t="s">
         <v>19</v>
       </c>
@@ -18113,7 +18128,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" ht="409.6">
       <c r="A71" s="1" t="s">
         <v>19</v>
       </c>
@@ -18154,7 +18169,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" ht="409.6">
       <c r="A72" s="1" t="s">
         <v>19</v>
       </c>
@@ -18195,7 +18210,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" ht="409.6">
       <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
@@ -18236,7 +18251,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A74" s="10" t="s">
         <v>19</v>
       </c>
@@ -18280,7 +18295,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A75" s="10" t="s">
         <v>19</v>
       </c>
@@ -18322,7 +18337,7 @@
       </c>
       <c r="N75" s="32"/>
     </row>
-    <row r="76" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A76" s="10" t="s">
         <v>19</v>
       </c>
@@ -18364,7 +18379,7 @@
       </c>
       <c r="N76" s="32"/>
     </row>
-    <row r="77" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A77" s="10" t="s">
         <v>19</v>
       </c>
@@ -18406,7 +18421,7 @@
       </c>
       <c r="N77" s="32"/>
     </row>
-    <row r="78" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A78" s="10" t="s">
         <v>19</v>
       </c>
@@ -18448,7 +18463,7 @@
       </c>
       <c r="N78" s="32"/>
     </row>
-    <row r="79" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" ht="409.6">
       <c r="A79" s="1" t="s">
         <v>19</v>
       </c>
@@ -18492,7 +18507,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" ht="409.6">
       <c r="A80" s="1" t="s">
         <v>19</v>
       </c>
@@ -18533,7 +18548,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" ht="409.6">
       <c r="A81" s="1" t="s">
         <v>19</v>
       </c>
@@ -18574,7 +18589,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" ht="409.6">
       <c r="A82" s="1" t="s">
         <v>19</v>
       </c>
@@ -18615,7 +18630,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" ht="409.6">
       <c r="A83" s="1" t="s">
         <v>19</v>
       </c>
@@ -18656,7 +18671,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="84" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A84" s="10" t="s">
         <v>19</v>
       </c>
@@ -18700,7 +18715,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A85" s="10" t="s">
         <v>19</v>
       </c>
@@ -18742,7 +18757,7 @@
       </c>
       <c r="N85" s="32"/>
     </row>
-    <row r="86" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A86" s="10" t="s">
         <v>19</v>
       </c>
@@ -18784,7 +18799,7 @@
       </c>
       <c r="N86" s="32"/>
     </row>
-    <row r="87" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A87" s="10" t="s">
         <v>19</v>
       </c>
@@ -18826,7 +18841,7 @@
       </c>
       <c r="N87" s="32"/>
     </row>
-    <row r="88" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A88" s="10" t="s">
         <v>19</v>
       </c>
@@ -18868,7 +18883,7 @@
       </c>
       <c r="N88" s="32"/>
     </row>
-    <row r="89" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" s="10" customFormat="1">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -18890,7 +18905,7 @@
       <c r="M89" s="14"/>
       <c r="N89" s="32"/>
     </row>
-    <row r="90" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" s="10" customFormat="1">
       <c r="A90" s="1" t="s">
         <v>19</v>
       </c>
@@ -18912,7 +18927,7 @@
       <c r="M90" s="14"/>
       <c r="N90" s="32"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" ht="16.5">
       <c r="A91" s="1" t="s">
         <v>19</v>
       </c>
@@ -18930,7 +18945,7 @@
       </c>
       <c r="K91" s="3"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" ht="16.5">
       <c r="A92" s="1" t="s">
         <v>19</v>
       </c>
@@ -18948,7 +18963,7 @@
       </c>
       <c r="K92" s="3"/>
     </row>
-    <row r="93" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A93" s="10" t="s">
         <v>334</v>
       </c>
@@ -18992,7 +19007,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="94" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A94" s="10" t="s">
         <v>334</v>
       </c>
@@ -19034,7 +19049,7 @@
       </c>
       <c r="N94" s="32"/>
     </row>
-    <row r="95" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A95" s="10" t="s">
         <v>334</v>
       </c>
@@ -19076,7 +19091,7 @@
       </c>
       <c r="N95" s="32"/>
     </row>
-    <row r="96" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A96" s="10" t="s">
         <v>334</v>
       </c>
@@ -19118,7 +19133,7 @@
       </c>
       <c r="N96" s="32"/>
     </row>
-    <row r="97" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A97" s="10" t="s">
         <v>334</v>
       </c>
@@ -19160,7 +19175,7 @@
       </c>
       <c r="N97" s="32"/>
     </row>
-    <row r="98" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" ht="409.6">
       <c r="A98" s="1" t="s">
         <v>334</v>
       </c>
@@ -19204,7 +19219,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" ht="409.6">
       <c r="A99" s="1" t="s">
         <v>334</v>
       </c>
@@ -19245,7 +19260,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14" ht="409.6">
       <c r="A100" s="1" t="s">
         <v>334</v>
       </c>
@@ -19286,7 +19301,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14" ht="409.6">
       <c r="A101" s="1" t="s">
         <v>334</v>
       </c>
@@ -19327,7 +19342,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="102" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A102" s="10" t="s">
         <v>334</v>
       </c>
@@ -19371,7 +19386,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="103" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A103" s="10" t="s">
         <v>334</v>
       </c>
@@ -19413,7 +19428,7 @@
       </c>
       <c r="N103" s="32"/>
     </row>
-    <row r="104" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A104" s="10" t="s">
         <v>334</v>
       </c>
@@ -19455,7 +19470,7 @@
       </c>
       <c r="N104" s="32"/>
     </row>
-    <row r="105" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A105" s="10" t="s">
         <v>334</v>
       </c>
@@ -19497,7 +19512,7 @@
       </c>
       <c r="N105" s="32"/>
     </row>
-    <row r="106" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:14" ht="409.6">
       <c r="A106" s="10" t="s">
         <v>334</v>
       </c>
@@ -19541,7 +19556,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:14" ht="409.6">
       <c r="A107" s="10" t="s">
         <v>334</v>
       </c>
@@ -19582,7 +19597,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:14" ht="409.6">
       <c r="A108" s="10" t="s">
         <v>334</v>
       </c>
@@ -19623,7 +19638,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:14" ht="409.6">
       <c r="A109" s="10" t="s">
         <v>334</v>
       </c>
@@ -19664,7 +19679,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:14" ht="409.6">
       <c r="A110" s="10" t="s">
         <v>334</v>
       </c>
@@ -19705,7 +19720,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="219" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:14" ht="219" customHeight="1">
       <c r="A111" s="1" t="s">
         <v>334</v>
       </c>
@@ -19749,7 +19764,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="219" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:14" ht="219" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>334</v>
       </c>
@@ -19790,7 +19805,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="219" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14" ht="219" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>334</v>
       </c>
@@ -19831,7 +19846,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="219" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14" ht="219" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>334</v>
       </c>
@@ -19872,7 +19887,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:14">
       <c r="A115" s="1" t="s">
         <v>334</v>
       </c>
@@ -19887,7 +19902,7 @@
       </c>
       <c r="K115" s="3"/>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14">
       <c r="A116" s="1" t="s">
         <v>334</v>
       </c>
@@ -19902,7 +19917,7 @@
       </c>
       <c r="K116" s="3"/>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14">
       <c r="A117" s="1" t="s">
         <v>334</v>
       </c>
@@ -19917,7 +19932,7 @@
       </c>
       <c r="K117" s="3"/>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14">
       <c r="A118" s="1" t="s">
         <v>334</v>
       </c>
@@ -19931,7 +19946,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14" ht="409.6">
       <c r="A119" s="1" t="s">
         <v>334</v>
       </c>
@@ -19975,7 +19990,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14" ht="409.6">
       <c r="A120" s="1" t="s">
         <v>334</v>
       </c>
@@ -20016,7 +20031,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14" ht="409.6">
       <c r="A121" s="1" t="s">
         <v>334</v>
       </c>
@@ -20057,7 +20072,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14" ht="409.6">
       <c r="A122" s="1" t="s">
         <v>334</v>
       </c>
@@ -20098,7 +20113,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14" ht="409.6">
       <c r="A123" s="1" t="s">
         <v>334</v>
       </c>
@@ -20139,7 +20154,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14" ht="201.95" customHeight="1">
       <c r="A124" s="1" t="s">
         <v>334</v>
       </c>
@@ -20183,7 +20198,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14" ht="201.95" customHeight="1">
       <c r="A125" s="1" t="s">
         <v>334</v>
       </c>
@@ -20224,7 +20239,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14" ht="201.95" customHeight="1">
       <c r="A126" s="1" t="s">
         <v>334</v>
       </c>
@@ -20265,7 +20280,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14" ht="201.95" customHeight="1">
       <c r="A127" s="1" t="s">
         <v>334</v>
       </c>
@@ -20306,7 +20321,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="202" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14" ht="201.95" customHeight="1">
       <c r="A128" s="1" t="s">
         <v>334</v>
       </c>
@@ -20347,7 +20362,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="129" spans="1:14" s="10" customFormat="1" ht="206.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14" s="10" customFormat="1" ht="206.1" customHeight="1">
       <c r="A129" s="10" t="s">
         <v>334</v>
       </c>
@@ -20391,7 +20406,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="130" spans="1:14" s="10" customFormat="1" ht="206.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14" s="10" customFormat="1" ht="206.1" customHeight="1">
       <c r="A130" s="10" t="s">
         <v>334</v>
       </c>
@@ -20433,7 +20448,7 @@
       </c>
       <c r="N130" s="32"/>
     </row>
-    <row r="131" spans="1:14" s="10" customFormat="1" ht="206.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14" s="10" customFormat="1" ht="206.1" customHeight="1">
       <c r="A131" s="10" t="s">
         <v>334</v>
       </c>
@@ -20475,7 +20490,7 @@
       </c>
       <c r="N131" s="32"/>
     </row>
-    <row r="132" spans="1:14" s="10" customFormat="1" ht="206.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14" s="10" customFormat="1" ht="206.1" customHeight="1">
       <c r="A132" s="10" t="s">
         <v>334</v>
       </c>
@@ -20517,7 +20532,7 @@
       </c>
       <c r="N132" s="32"/>
     </row>
-    <row r="133" spans="1:14" s="10" customFormat="1" ht="206.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14" s="10" customFormat="1" ht="206.1" customHeight="1">
       <c r="A133" s="10" t="s">
         <v>334</v>
       </c>
@@ -20559,7 +20574,7 @@
       </c>
       <c r="N133" s="32"/>
     </row>
-    <row r="134" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14" ht="409.6">
       <c r="A134" s="1" t="s">
         <v>334</v>
       </c>
@@ -20603,7 +20618,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" ht="409.6">
       <c r="A135" s="1" t="s">
         <v>334</v>
       </c>
@@ -20644,7 +20659,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" ht="409.6">
       <c r="A136" s="1" t="s">
         <v>334</v>
       </c>
@@ -20685,7 +20700,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14" ht="409.6">
       <c r="A137" s="1" t="s">
         <v>334</v>
       </c>
@@ -20726,7 +20741,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14" ht="409.6">
       <c r="A138" s="1" t="s">
         <v>334</v>
       </c>
@@ -20767,7 +20782,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="139" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A139" s="1" t="s">
         <v>334</v>
       </c>
@@ -20811,7 +20826,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="140" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A140" s="1" t="s">
         <v>334</v>
       </c>
@@ -20853,7 +20868,7 @@
       </c>
       <c r="N140" s="32"/>
     </row>
-    <row r="141" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A141" s="1" t="s">
         <v>334</v>
       </c>
@@ -20895,7 +20910,7 @@
       </c>
       <c r="N141" s="32"/>
     </row>
-    <row r="142" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A142" s="1" t="s">
         <v>334</v>
       </c>
@@ -20937,7 +20952,7 @@
       </c>
       <c r="N142" s="32"/>
     </row>
-    <row r="143" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A143" s="1" t="s">
         <v>334</v>
       </c>
@@ -20979,7 +20994,7 @@
       </c>
       <c r="N143" s="32"/>
     </row>
-    <row r="146" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:14" ht="409.6">
       <c r="A146" s="1" t="s">
         <v>334</v>
       </c>
@@ -21023,7 +21038,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" ht="409.6">
       <c r="A147" s="1" t="s">
         <v>334</v>
       </c>
@@ -21064,7 +21079,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14" ht="409.6">
       <c r="A148" s="1" t="s">
         <v>334</v>
       </c>
@@ -21105,7 +21120,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14" ht="409.6">
       <c r="A149" s="1" t="s">
         <v>334</v>
       </c>
@@ -21146,7 +21161,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" ht="409.6">
       <c r="A150" s="1" t="s">
         <v>334</v>
       </c>
@@ -21187,7 +21202,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="151" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A151" s="10" t="s">
         <v>334</v>
       </c>
@@ -21231,7 +21246,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="152" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A152" s="10" t="s">
         <v>334</v>
       </c>
@@ -21273,7 +21288,7 @@
       </c>
       <c r="N152" s="32"/>
     </row>
-    <row r="153" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A153" s="10" t="s">
         <v>334</v>
       </c>
@@ -21310,12 +21325,12 @@
       <c r="L153" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="M153" s="14" t="s">
+      <c r="M153" s="37" t="s">
         <v>547</v>
       </c>
       <c r="N153" s="32"/>
     </row>
-    <row r="154" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A154" s="10" t="s">
         <v>334</v>
       </c>
@@ -21357,7 +21372,7 @@
       </c>
       <c r="N154" s="32"/>
     </row>
-    <row r="155" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A155" s="10" t="s">
         <v>334</v>
       </c>
@@ -21401,7 +21416,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="156" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A156" s="10" t="s">
         <v>334</v>
       </c>
@@ -21443,7 +21458,7 @@
       </c>
       <c r="N156" s="32"/>
     </row>
-    <row r="157" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A157" s="10" t="s">
         <v>334</v>
       </c>
@@ -21485,7 +21500,7 @@
       </c>
       <c r="N157" s="32"/>
     </row>
-    <row r="158" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A158" s="10" t="s">
         <v>334</v>
       </c>
@@ -21527,7 +21542,7 @@
       </c>
       <c r="N158" s="32"/>
     </row>
-    <row r="159" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A159" s="10" t="s">
         <v>334</v>
       </c>
@@ -21569,7 +21584,7 @@
       </c>
       <c r="N159" s="32"/>
     </row>
-    <row r="160" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A160" s="10" t="s">
         <v>334</v>
       </c>
@@ -21613,7 +21628,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="161" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A161" s="10" t="s">
         <v>334</v>
       </c>
@@ -21655,7 +21670,7 @@
       </c>
       <c r="N161" s="32"/>
     </row>
-    <row r="162" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A162" s="10" t="s">
         <v>334</v>
       </c>
@@ -21697,7 +21712,7 @@
       </c>
       <c r="N162" s="32"/>
     </row>
-    <row r="163" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A163" s="10" t="s">
         <v>334</v>
       </c>
@@ -21739,7 +21754,7 @@
       </c>
       <c r="N163" s="32"/>
     </row>
-    <row r="164" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A164" s="10" t="s">
         <v>334</v>
       </c>
@@ -21781,7 +21796,7 @@
       </c>
       <c r="N164" s="32"/>
     </row>
-    <row r="165" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A165" s="10" t="s">
         <v>334</v>
       </c>
@@ -21825,7 +21840,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="166" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A166" s="10" t="s">
         <v>334</v>
       </c>
@@ -21867,7 +21882,7 @@
       </c>
       <c r="N166" s="32"/>
     </row>
-    <row r="167" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A167" s="10" t="s">
         <v>334</v>
       </c>
@@ -21909,7 +21924,7 @@
       </c>
       <c r="N167" s="32"/>
     </row>
-    <row r="168" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A168" s="10" t="s">
         <v>334</v>
       </c>
@@ -21951,7 +21966,7 @@
       </c>
       <c r="N168" s="32"/>
     </row>
-    <row r="169" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A169" s="10" t="s">
         <v>334</v>
       </c>
@@ -21993,7 +22008,7 @@
       </c>
       <c r="N169" s="32"/>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:14">
       <c r="A170" s="1" t="s">
         <v>334</v>
       </c>
@@ -22008,7 +22023,7 @@
       </c>
       <c r="K170" s="3"/>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:14">
       <c r="A171" s="1" t="s">
         <v>334</v>
       </c>
@@ -22023,7 +22038,7 @@
       </c>
       <c r="K171" s="3"/>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:14">
       <c r="A172" s="1" t="s">
         <v>334</v>
       </c>
@@ -22038,7 +22053,7 @@
       </c>
       <c r="K172" s="3"/>
     </row>
-    <row r="173" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:14" ht="409.6">
       <c r="A173" s="1" t="s">
         <v>607</v>
       </c>
@@ -22082,7 +22097,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:14" ht="409.6">
       <c r="A174" s="1" t="s">
         <v>607</v>
       </c>
@@ -22123,7 +22138,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:14" ht="409.6">
       <c r="A175" s="1" t="s">
         <v>607</v>
       </c>
@@ -22164,7 +22179,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:14" ht="409.6">
       <c r="A176" s="1" t="s">
         <v>607</v>
       </c>
@@ -22205,7 +22220,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:14" ht="409.6">
       <c r="A177" s="1" t="s">
         <v>607</v>
       </c>
@@ -22249,7 +22264,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:14" ht="409.6">
       <c r="A178" s="1" t="s">
         <v>607</v>
       </c>
@@ -22290,7 +22305,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:14" ht="409.6">
       <c r="A179" s="1" t="s">
         <v>607</v>
       </c>
@@ -22331,7 +22346,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:14" ht="409.6">
       <c r="A180" s="1" t="s">
         <v>607</v>
       </c>
@@ -22372,7 +22387,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="181" spans="1:14" s="10" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:14" s="10" customFormat="1" ht="222.95" customHeight="1">
       <c r="A181" s="10" t="s">
         <v>607</v>
       </c>
@@ -22416,7 +22431,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="182" spans="1:14" s="10" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:14" s="10" customFormat="1" ht="222.95" customHeight="1">
       <c r="A182" s="10" t="s">
         <v>607</v>
       </c>
@@ -22458,7 +22473,7 @@
       </c>
       <c r="N182" s="32"/>
     </row>
-    <row r="183" spans="1:14" s="10" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:14" s="10" customFormat="1" ht="222.95" customHeight="1">
       <c r="A183" s="10" t="s">
         <v>607</v>
       </c>
@@ -22500,7 +22515,7 @@
       </c>
       <c r="N183" s="32"/>
     </row>
-    <row r="184" spans="1:14" s="10" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:14" s="10" customFormat="1" ht="222.95" customHeight="1">
       <c r="A184" s="10" t="s">
         <v>607</v>
       </c>
@@ -22542,7 +22557,7 @@
       </c>
       <c r="N184" s="32"/>
     </row>
-    <row r="185" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A185" s="10" t="s">
         <v>607</v>
       </c>
@@ -22586,7 +22601,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="186" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A186" s="10" t="s">
         <v>607</v>
       </c>
@@ -22628,7 +22643,7 @@
       </c>
       <c r="N186" s="32"/>
     </row>
-    <row r="187" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A187" s="10" t="s">
         <v>607</v>
       </c>
@@ -22670,7 +22685,7 @@
       </c>
       <c r="N187" s="32"/>
     </row>
-    <row r="188" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A188" s="10" t="s">
         <v>607</v>
       </c>
@@ -22712,7 +22727,7 @@
       </c>
       <c r="N188" s="32"/>
     </row>
-    <row r="189" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A189" s="10" t="s">
         <v>607</v>
       </c>
@@ -22754,7 +22769,7 @@
       </c>
       <c r="N189" s="32"/>
     </row>
-    <row r="190" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A190" s="10" t="s">
         <v>607</v>
       </c>
@@ -22798,7 +22813,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="191" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A191" s="10" t="s">
         <v>607</v>
       </c>
@@ -22840,7 +22855,7 @@
       </c>
       <c r="N191" s="32"/>
     </row>
-    <row r="192" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A192" s="10" t="s">
         <v>607</v>
       </c>
@@ -22882,7 +22897,7 @@
       </c>
       <c r="N192" s="32"/>
     </row>
-    <row r="193" spans="1:14" s="10" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:14" s="10" customFormat="1" ht="409.6">
       <c r="A193" s="10" t="s">
         <v>607</v>
       </c>
@@ -22924,7 +22939,7 @@
       </c>
       <c r="N193" s="32"/>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:14">
       <c r="A194" s="1" t="s">
         <v>607</v>
       </c>
@@ -22939,7 +22954,7 @@
       </c>
       <c r="M194" s="1"/>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:14">
       <c r="A195" s="1" t="s">
         <v>607</v>
       </c>
@@ -22953,7 +22968,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:14">
       <c r="A196" s="1" t="s">
         <v>607</v>
       </c>
@@ -22967,7 +22982,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:14">
       <c r="A197" s="1" t="s">
         <v>607</v>
       </c>

</xml_diff>